<commit_message>
update for file path copies
</commit_message>
<xml_diff>
--- a/runs/osu867/ncbi_mapping/ncbi_submission_data/has_biosamp_accession/has_biosamp_accession_osu867_SRA_metadata.xlsx
+++ b/runs/osu867/ncbi_mapping/ncbi_submission_data/has_biosamp_accession/has_biosamp_accession_osu867_SRA_metadata.xlsx
@@ -1384,7 +1384,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K2" s="11" t="inlineStr">
@@ -1394,12 +1394,12 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>MP_E25_2B_DY20_R1.fastq.gz</t>
+          <t>E25.2B.DY20-12_Parada16S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>MP_E25_2B_DY20_R2.fastq.gz</t>
+          <t>E25.2B.DY20-12_Parada16S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
@@ -1461,7 +1461,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K3" s="11" t="inlineStr">
@@ -1471,12 +1471,12 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>MP_E26_1B_DY20_R1.fastq.gz</t>
+          <t>E26.1B.DY20-12_Parada16S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>MP_E26_1B_DY20_R2.fastq.gz</t>
+          <t>E26.1B.DY20-12_Parada16S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
@@ -1538,7 +1538,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K4" s="11" t="inlineStr">
@@ -1548,12 +1548,12 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>MP_E27_1B_DY20_R1.fastq.gz</t>
+          <t>E27.1B.DY20-12_Parada16S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>MP_E27_1B_DY20_R2.fastq.gz</t>
+          <t>E27.1B.DY20-12_Parada16S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
@@ -1615,7 +1615,7 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K5" s="11" t="inlineStr">
@@ -1625,12 +1625,12 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>MP_E27_2B_DY20_R1.fastq.gz</t>
+          <t>E27.2B.DY20-12_Parada16S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>MP_E27_2B_DY20_R2.fastq.gz</t>
+          <t>E27.2B.DY20-12_Parada16S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
@@ -1692,7 +1692,7 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K6" s="11" t="inlineStr">
@@ -1702,12 +1702,12 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>MP_E28_1B_DY20_R1.fastq.gz</t>
+          <t>E28.1B.DY20-12_Parada16S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>MP_E28_1B_DY20_R2.fastq.gz</t>
+          <t>E28.1B.DY20-12_Parada16S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
@@ -1769,7 +1769,7 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K7" s="11" t="inlineStr">
@@ -1779,12 +1779,12 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>MP_E29_1B_DY20_R1.fastq.gz</t>
+          <t>E29.1B.DY20-12_Parada16S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>MP_E29_1B_DY20_R2.fastq.gz</t>
+          <t>E29.1B.DY20-12_Parada16S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
@@ -1846,7 +1846,7 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K8" s="11" t="inlineStr">
@@ -1856,12 +1856,12 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>MP_E30_1B_DY20_R1.fastq.gz</t>
+          <t>E30.1B.DY20-12_Parada16S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>MP_E30_1B_DY20_R2.fastq.gz</t>
+          <t>E30.1B.DY20-12_Parada16S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
@@ -1923,7 +1923,7 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K9" s="11" t="inlineStr">
@@ -1933,12 +1933,12 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>MP_E31_1B_DY20_R1.fastq.gz</t>
+          <t>E31.1B.DY20-12_Parada16S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>MP_E31_1B_DY20_R2.fastq.gz</t>
+          <t>E31.1B.DY20-12_Parada16S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
@@ -2000,7 +2000,7 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K10" s="11" t="inlineStr">
@@ -2010,12 +2010,12 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>MP_E32_1B_DY20_R1.fastq.gz</t>
+          <t>E32.1B.DY20-12_Parada16S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>MP_E32_1B_DY20_R2.fastq.gz</t>
+          <t>E32.1B.DY20-12_Parada16S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
@@ -2077,7 +2077,7 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K11" s="11" t="inlineStr">
@@ -2087,12 +2087,12 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>MP_E33_1B_DY20_R1.fastq.gz</t>
+          <t>E33.1B.DY20-12_Parada16S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>MP_E33_1B_DY20_R2.fastq.gz</t>
+          <t>E33.1B.DY20-12_Parada16S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
@@ -2154,7 +2154,7 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K12" s="11" t="inlineStr">
@@ -2164,12 +2164,12 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>MP_E34_1B_DY20_R1.fastq.gz</t>
+          <t>E34.1B.DY20-12_Parada16S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>MP_E34_1B_DY20_R2.fastq.gz</t>
+          <t>E34.1B.DY20-12_Parada16S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
@@ -2231,7 +2231,7 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K13" s="11" t="inlineStr">
@@ -2241,12 +2241,12 @@
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>MP_E35_1B_DY20_R1.fastq.gz</t>
+          <t>E35.1B.DY20-12_Parada16S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>MP_E35_1B_DY20_R2.fastq.gz</t>
+          <t>E35.1B.DY20-12_Parada16S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
@@ -2308,7 +2308,7 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K14" s="11" t="inlineStr">
@@ -2318,12 +2318,12 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>MP_E36_1B_DY20_R1.fastq.gz</t>
+          <t>E36.1B.DY20-12_Parada16S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>MP_E36_1B_DY20_R2.fastq.gz</t>
+          <t>E36.1B.DY20-12_Parada16S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
@@ -2385,7 +2385,7 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K15" s="11" t="inlineStr">
@@ -2395,12 +2395,12 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>MP_E36_2B_DY20_R1.fastq.gz</t>
+          <t>E36.2B.DY20-12_Parada16S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>MP_E36_2B_DY20_R2.fastq.gz</t>
+          <t>E36.2B.DY20-12_Parada16S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R15" t="inlineStr">
@@ -2462,7 +2462,7 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K16" s="11" t="inlineStr">
@@ -2472,12 +2472,12 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>MP_E37_1B_DY20_R1.fastq.gz</t>
+          <t>E37.1B.DY20-12_Parada16S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>MP_E37_1B_DY20_R2.fastq.gz</t>
+          <t>E37.1B.DY20-12_Parada16S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R16" t="inlineStr">
@@ -2539,7 +2539,7 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K17" s="11" t="inlineStr">
@@ -2549,12 +2549,12 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>MP_E38_1B_DY20_R1.fastq.gz</t>
+          <t>E38.1B.DY20-12_Parada16S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>MP_E38_1B_DY20_R2.fastq.gz</t>
+          <t>E38.1B.DY20-12_Parada16S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R17" t="inlineStr">
@@ -2616,7 +2616,7 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K18" s="11" t="inlineStr">
@@ -2626,12 +2626,12 @@
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>MP_E39_1B_DY20_R1.fastq.gz</t>
+          <t>E39.1B.DY20-12_Parada16S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>MP_E39_1B_DY20_R2.fastq.gz</t>
+          <t>E39.1B.DY20-12_Parada16S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R18" t="inlineStr">
@@ -2693,7 +2693,7 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K19" s="11" t="inlineStr">
@@ -2703,12 +2703,12 @@
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>MP_E40_1B_DY20_R1.fastq.gz</t>
+          <t>E40.1B.DY20-12_Parada16S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>MP_E40_1B_DY20_R2.fastq.gz</t>
+          <t>E40.1B.DY20-12_Parada16S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R19" t="inlineStr">
@@ -2770,7 +2770,7 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K20" s="11" t="inlineStr">
@@ -2780,12 +2780,12 @@
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>MP_E42_1B_DY20_R1.fastq.gz</t>
+          <t>E42.1B.DY20-12_Parada16S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>MP_E42_1B_DY20_R2.fastq.gz</t>
+          <t>E42.1B.DY20-12_Parada16S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R20" t="inlineStr">
@@ -2847,7 +2847,7 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K21" s="11" t="inlineStr">
@@ -2857,12 +2857,12 @@
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>MP_E43_1B_DY20_R1.fastq.gz</t>
+          <t>E43.1B.DY20-12_Parada16S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>MP_E43_1B_DY20_R2.fastq.gz</t>
+          <t>E43.1B.DY20-12_Parada16S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R21" t="inlineStr">
@@ -2924,7 +2924,7 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K22" s="11" t="inlineStr">
@@ -2934,12 +2934,12 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>MP_E44_DY20_R1.fastq.gz</t>
+          <t>E44.DY20-12_Parada16S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>MP_E44_DY20_R2.fastq.gz</t>
+          <t>E44.DY20-12_Parada16S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R22" t="inlineStr">
@@ -3001,7 +3001,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K23" s="11" t="inlineStr">
@@ -3011,12 +3011,12 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>MP_E45_1B_DY20_R1.fastq.gz</t>
+          <t>E45.1B.DY20-12_Parada16S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>MP_E45_1B_DY20_R2.fastq.gz</t>
+          <t>E45.1B.DY20-12_Parada16S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R23" t="inlineStr">
@@ -3078,7 +3078,7 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K24" s="11" t="inlineStr">
@@ -3088,12 +3088,12 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>MP_E46_1B_DY20_R1.fastq.gz</t>
+          <t>E46.1B.DY20-12_Parada16S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>MP_E46_1B_DY20_R2.fastq.gz</t>
+          <t>E46.1B.DY20-12_Parada16S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R24" t="inlineStr">
@@ -3155,7 +3155,7 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K25" s="11" t="inlineStr">
@@ -3165,12 +3165,12 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>MP_E46_2B_DY20_R1.fastq.gz</t>
+          <t>E46.2B.DY20-12_Parada16S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>MP_E46_2B_DY20_R2.fastq.gz</t>
+          <t>E46.2B.DY20-12_Parada16S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R25" t="inlineStr">
@@ -3232,7 +3232,7 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K26" s="11" t="inlineStr">
@@ -3242,12 +3242,12 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>MP_E47_1B_DY20_R1.fastq.gz</t>
+          <t>E47.1B.DY20-12_Parada16S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>MP_E47_1B_DY20_R2.fastq.gz</t>
+          <t>E47.1B.DY20-12_Parada16S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R26" t="inlineStr">
@@ -3309,7 +3309,7 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K27" s="11" t="inlineStr">
@@ -3319,12 +3319,12 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>MP_E48_1B_DY20_R1.fastq.gz</t>
+          <t>E48.1B.DY20-12_Parada16S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>MP_E48_1B_DY20_R2.fastq.gz</t>
+          <t>E48.1B.DY20-12_Parada16S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R27" t="inlineStr">
@@ -3386,7 +3386,7 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K28" s="11" t="inlineStr">
@@ -3396,12 +3396,12 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>MP_E49_1B_DY20_R1.fastq.gz</t>
+          <t>E49.1B.DY20-12_Parada16S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>MP_E49_1B_DY20_R2.fastq.gz</t>
+          <t>E49.1B.DY20-12_Parada16S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R28" t="inlineStr">
@@ -3463,7 +3463,7 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K29" s="11" t="inlineStr">
@@ -3473,12 +3473,12 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>MP_E49_2B_DY20_R1.fastq.gz</t>
+          <t>E49.2B.DY20-12_Parada16S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M29" t="inlineStr">
         <is>
-          <t>MP_E49_2B_DY20_R2.fastq.gz</t>
+          <t>E49.2B.DY20-12_Parada16S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R29" t="inlineStr">
@@ -3540,7 +3540,7 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K30" s="11" t="inlineStr">
@@ -3550,12 +3550,12 @@
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>MP_E50_1B_DY20_R1.fastq.gz</t>
+          <t>E50.1B.DY20-12_Parada16S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M30" t="inlineStr">
         <is>
-          <t>MP_E50_1B_DY20_R2.fastq.gz</t>
+          <t>E50.1B.DY20-12_Parada16S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R30" t="inlineStr">
@@ -3617,7 +3617,7 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K31" s="11" t="inlineStr">
@@ -3627,12 +3627,12 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>MP_E51_1B_DY20_R1.fastq.gz</t>
+          <t>E51.1B.DY20-12_Parada16S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>MP_E51_1B_DY20_R2.fastq.gz</t>
+          <t>E51.1B.DY20-12_Parada16S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R31" t="inlineStr">
@@ -3694,7 +3694,7 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K32" s="11" t="inlineStr">
@@ -3704,12 +3704,12 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>MP_E52_1B_DY20_R1.fastq.gz</t>
+          <t>E52.1B.DY20-12_Parada16S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>MP_E52_1B_DY20_R2.fastq.gz</t>
+          <t>E52.1B.DY20-12_Parada16S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R32" t="inlineStr">
@@ -3771,7 +3771,7 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K33" s="11" t="inlineStr">
@@ -3781,12 +3781,12 @@
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>MP_E53_1B_DY20_R1.fastq.gz</t>
+          <t>E53.1B.DY20-12_Parada16S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M33" t="inlineStr">
         <is>
-          <t>MP_E53_1B_DY20_R2.fastq.gz</t>
+          <t>E53.1B.DY20-12_Parada16S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R33" t="inlineStr">
@@ -3848,7 +3848,7 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K34" s="11" t="inlineStr">
@@ -3858,12 +3858,12 @@
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>MP_E53_2B_DY20_R1.fastq.gz</t>
+          <t>E53.2B.DY20-12_Parada16S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M34" t="inlineStr">
         <is>
-          <t>MP_E53_2B_DY20_R2.fastq.gz</t>
+          <t>E53.2B.DY20-12_Parada16S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R34" t="inlineStr">
@@ -3925,7 +3925,7 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K35" s="11" t="inlineStr">
@@ -3935,12 +3935,12 @@
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>MP_E54_1B_DY20_R1.fastq.gz</t>
+          <t>E54.1B.DY20-12_Parada16S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M35" t="inlineStr">
         <is>
-          <t>MP_E54_1B_DY20_R2.fastq.gz</t>
+          <t>E54.1B.DY20-12_Parada16S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R35" t="inlineStr">
@@ -4002,7 +4002,7 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K36" s="11" t="inlineStr">
@@ -4012,12 +4012,12 @@
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>MP_E54_2B_DY20_R1.fastq.gz</t>
+          <t>E54.2B.DY20-12_Parada16S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M36" t="inlineStr">
         <is>
-          <t>MP_E54_2B_DY20_R2.fastq.gz</t>
+          <t>E54.2B.DY20-12_Parada16S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R36" t="inlineStr">
@@ -4079,7 +4079,7 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K37" s="11" t="inlineStr">
@@ -4089,12 +4089,12 @@
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>MP_E55_1B_DY20_R1.fastq.gz</t>
+          <t>E55.1B.DY20-12_Parada16S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M37" t="inlineStr">
         <is>
-          <t>MP_E55_1B_DY20_R2.fastq.gz</t>
+          <t>E55.1B.DY20-12_Parada16S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R37" t="inlineStr">
@@ -4156,7 +4156,7 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K38" s="11" t="inlineStr">
@@ -4166,12 +4166,12 @@
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>MP_E57_1B_DY20_R1.fastq.gz</t>
+          <t>E57.1B.DY20-12_Parada16S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M38" t="inlineStr">
         <is>
-          <t>MP_E57_1B_DY20_R2.fastq.gz</t>
+          <t>E57.1B.DY20-12_Parada16S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R38" t="inlineStr">
@@ -4233,7 +4233,7 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K39" s="11" t="inlineStr">
@@ -4243,12 +4243,12 @@
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>MP_E58_1B_DY20_R1.fastq.gz</t>
+          <t>E58.1B.DY20-12_Parada16S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M39" t="inlineStr">
         <is>
-          <t>MP_E58_1B_DY20_R2.fastq.gz</t>
+          <t>E58.1B.DY20-12_Parada16S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R39" t="inlineStr">
@@ -4310,7 +4310,7 @@
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K40" s="11" t="inlineStr">
@@ -4320,12 +4320,12 @@
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>MP_E58_2B_DY20_R1.fastq.gz</t>
+          <t>E58.2B.DY20-12_Parada16S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M40" t="inlineStr">
         <is>
-          <t>MP_E58_2B_DY20_R2.fastq.gz</t>
+          <t>E58.2B.DY20-12_Parada16S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R40" t="inlineStr">
@@ -4387,7 +4387,7 @@
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K41" s="11" t="inlineStr">
@@ -4397,12 +4397,12 @@
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>MP_E59_1B_DY20_R1.fastq.gz</t>
+          <t>E59.1B.DY20-12_Parada16S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>MP_E59_1B_DY20_R2.fastq.gz</t>
+          <t>E59.1B.DY20-12_Parada16S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R41" t="inlineStr">
@@ -4464,7 +4464,7 @@
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K42" s="11" t="inlineStr">
@@ -4474,12 +4474,12 @@
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>MP_E60_1B_DY20_R1.fastq.gz</t>
+          <t>E60.1B.DY20-12_Parada16S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M42" t="inlineStr">
         <is>
-          <t>MP_E60_1B_DY20_R2.fastq.gz</t>
+          <t>E60.1B.DY20-12_Parada16S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R42" t="inlineStr">
@@ -4541,7 +4541,7 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K43" s="11" t="inlineStr">
@@ -4551,12 +4551,12 @@
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>MP_E61_1B_DY20_R1.fastq.gz</t>
+          <t>E61.1B.DY20-12_Parada16S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M43" t="inlineStr">
         <is>
-          <t>MP_E61_1B_DY20_R2.fastq.gz</t>
+          <t>E61.1B.DY20-12_Parada16S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R43" t="inlineStr">
@@ -4618,7 +4618,7 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K44" s="11" t="inlineStr">
@@ -4628,12 +4628,12 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>MP_E62_1B_DY20_R1.fastq.gz</t>
+          <t>E62.1B.DY20-12_Parada16S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M44" t="inlineStr">
         <is>
-          <t>MP_E62_1B_DY20_R2.fastq.gz</t>
+          <t>E62.1B.DY20-12_Parada16S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R44" t="inlineStr">
@@ -4695,7 +4695,7 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K45" s="11" t="inlineStr">
@@ -4705,12 +4705,12 @@
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>MP_E63_1B_DY20_R1.fastq.gz</t>
+          <t>E63.1B.DY20-12_Parada16S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M45" t="inlineStr">
         <is>
-          <t>MP_E63_1B_DY20_R2.fastq.gz</t>
+          <t>E63.1B.DY20-12_Parada16S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R45" t="inlineStr">
@@ -4772,7 +4772,7 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K46" s="11" t="inlineStr">
@@ -4782,12 +4782,12 @@
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>MP_E64_1B_DY20_R1.fastq.gz</t>
+          <t>E64.1B.DY20-12_Parada16S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M46" t="inlineStr">
         <is>
-          <t>MP_E64_1B_DY20_R2.fastq.gz</t>
+          <t>E64.1B.DY20-12_Parada16S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R46" t="inlineStr">
@@ -4849,7 +4849,7 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K47" s="11" t="inlineStr">
@@ -4859,12 +4859,12 @@
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>MP_E65_1B_DY20_R1.fastq.gz</t>
+          <t>E65.1B.DY20-12_Parada16S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M47" t="inlineStr">
         <is>
-          <t>MP_E65_1B_DY20_R2.fastq.gz</t>
+          <t>E65.1B.DY20-12_Parada16S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R47" t="inlineStr">
@@ -4926,7 +4926,7 @@
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K48" s="11" t="inlineStr">
@@ -4936,12 +4936,12 @@
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>MP_E66_1B_DY20_R1.fastq.gz</t>
+          <t>E66.1B.DY20-12_Parada16S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M48" t="inlineStr">
         <is>
-          <t>MP_E66_1B_DY20_R2.fastq.gz</t>
+          <t>E66.1B.DY20-12_Parada16S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R48" t="inlineStr">
@@ -5003,7 +5003,7 @@
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K49" s="11" t="inlineStr">
@@ -5013,12 +5013,12 @@
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>MP_E67_1B_DY20_R1.fastq.gz</t>
+          <t>E67.1B.DY20-12_Parada16S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M49" t="inlineStr">
         <is>
-          <t>MP_E67_1B_DY20_R2.fastq.gz</t>
+          <t>E67.1B.DY20-12_Parada16S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R49" t="inlineStr">
@@ -5080,7 +5080,7 @@
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K50" s="11" t="inlineStr">
@@ -5090,12 +5090,12 @@
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>MP_E68_1B_DY20_R1.fastq.gz</t>
+          <t>E68.1B.DY20-12_Parada16S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M50" t="inlineStr">
         <is>
-          <t>MP_E68_1B_DY20_R2.fastq.gz</t>
+          <t>E68.1B.DY20-12_Parada16S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R50" t="inlineStr">
@@ -5157,7 +5157,7 @@
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K51" s="11" t="inlineStr">
@@ -5167,12 +5167,12 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>MP_E69_1B_DY20_R1.fastq.gz</t>
+          <t>E69.1B.DY20-12_Parada16S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M51" t="inlineStr">
         <is>
-          <t>MP_E69_1B_DY20_R2.fastq.gz</t>
+          <t>E69.1B.DY20-12_Parada16S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R51" t="inlineStr">
@@ -5234,7 +5234,7 @@
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K52" s="11" t="inlineStr">
@@ -5244,12 +5244,12 @@
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>MP_E70_1B_DY20_R1.fastq.gz</t>
+          <t>E70.1B.DY20-12_Parada16S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M52" t="inlineStr">
         <is>
-          <t>MP_E70_1B_DY20_R2.fastq.gz</t>
+          <t>E70.1B.DY20-12_Parada16S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R52" t="inlineStr">
@@ -5311,7 +5311,7 @@
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K53" s="11" t="inlineStr">
@@ -5321,12 +5321,12 @@
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>MP_E71_1B_DY20_R1.fastq.gz</t>
+          <t>E71.1B.DY20-12_Parada16S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M53" t="inlineStr">
         <is>
-          <t>MP_E71_1B_DY20_R2.fastq.gz</t>
+          <t>E71.1B.DY20-12_Parada16S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R53" t="inlineStr">
@@ -5388,7 +5388,7 @@
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K54" s="11" t="inlineStr">
@@ -5398,12 +5398,12 @@
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>MP_E72_1B_DY20_R1.fastq.gz</t>
+          <t>E72.1B.DY20-12_Parada16S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M54" t="inlineStr">
         <is>
-          <t>MP_E72_1B_DY20_R2.fastq.gz</t>
+          <t>E72.1B.DY20-12_Parada16S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R54" t="inlineStr">
@@ -5465,7 +5465,7 @@
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K55" s="11" t="inlineStr">
@@ -5475,12 +5475,12 @@
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>MP_E25_2B_DY20_R1.fastq.gz</t>
+          <t>E25.2B.DY20-12_Machida18S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M55" t="inlineStr">
         <is>
-          <t>MP_E25_2B_DY20_R2.fastq.gz</t>
+          <t>E25.2B.DY20-12_Machida18S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R55" t="inlineStr">
@@ -5542,7 +5542,7 @@
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K56" s="11" t="inlineStr">
@@ -5552,12 +5552,12 @@
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>MP_E26_1B_DY20_R1.fastq.gz</t>
+          <t>E26.1B.DY20-12_Machida18S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M56" t="inlineStr">
         <is>
-          <t>MP_E26_1B_DY20_R2.fastq.gz</t>
+          <t>E26.1B.DY20-12_Machida18S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R56" t="inlineStr">
@@ -5619,7 +5619,7 @@
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K57" s="11" t="inlineStr">
@@ -5629,12 +5629,12 @@
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>MP_E27_1B_DY20_R1.fastq.gz</t>
+          <t>E27.1B.DY20-12_Machida18S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M57" t="inlineStr">
         <is>
-          <t>MP_E27_1B_DY20_R2.fastq.gz</t>
+          <t>E27.1B.DY20-12_Machida18S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R57" t="inlineStr">
@@ -5691,7 +5691,7 @@
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K58" s="11" t="inlineStr">
@@ -5701,12 +5701,12 @@
       </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>MP_E27_2B_DY20_R1.fastq.gz</t>
+          <t>E27.2B.DY20-12_Machida18S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M58" t="inlineStr">
         <is>
-          <t>MP_E27_2B_DY20_R2.fastq.gz</t>
+          <t>E27.2B.DY20-12_Machida18S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R58" t="inlineStr">
@@ -5768,7 +5768,7 @@
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K59" s="11" t="inlineStr">
@@ -5778,12 +5778,12 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>MP_E28_1B_DY20_R1.fastq.gz</t>
+          <t>E28.1B.DY20-12_Machida18S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M59" t="inlineStr">
         <is>
-          <t>MP_E28_1B_DY20_R2.fastq.gz</t>
+          <t>E28.1B.DY20-12_Machida18S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R59" t="inlineStr">
@@ -5845,7 +5845,7 @@
       </c>
       <c r="J60" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K60" s="11" t="inlineStr">
@@ -5855,12 +5855,12 @@
       </c>
       <c r="L60" t="inlineStr">
         <is>
-          <t>MP_E29_1B_DY20_R1.fastq.gz</t>
+          <t>E29.1B.DY20-12_Machida18S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M60" t="inlineStr">
         <is>
-          <t>MP_E29_1B_DY20_R2.fastq.gz</t>
+          <t>E29.1B.DY20-12_Machida18S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R60" t="inlineStr">
@@ -5922,7 +5922,7 @@
       </c>
       <c r="J61" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K61" s="11" t="inlineStr">
@@ -5932,12 +5932,12 @@
       </c>
       <c r="L61" t="inlineStr">
         <is>
-          <t>MP_E30_1B_DY20_R1.fastq.gz</t>
+          <t>E30.1B.DY20-12_Machida18S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M61" t="inlineStr">
         <is>
-          <t>MP_E30_1B_DY20_R2.fastq.gz</t>
+          <t>E30.1B.DY20-12_Machida18S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R61" t="inlineStr">
@@ -5999,7 +5999,7 @@
       </c>
       <c r="J62" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K62" s="11" t="inlineStr">
@@ -6009,12 +6009,12 @@
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>MP_E31_1B_DY20_R1.fastq.gz</t>
+          <t>E31.1B.DY20-12_Machida18S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M62" t="inlineStr">
         <is>
-          <t>MP_E31_1B_DY20_R2.fastq.gz</t>
+          <t>E31.1B.DY20-12_Machida18S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R62" t="inlineStr">
@@ -6076,7 +6076,7 @@
       </c>
       <c r="J63" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K63" s="11" t="inlineStr">
@@ -6086,12 +6086,12 @@
       </c>
       <c r="L63" t="inlineStr">
         <is>
-          <t>MP_E32_1B_DY20_R1.fastq.gz</t>
+          <t>E32.1B.DY20-12_Machida18S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M63" t="inlineStr">
         <is>
-          <t>MP_E32_1B_DY20_R2.fastq.gz</t>
+          <t>E32.1B.DY20-12_Machida18S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R63" t="inlineStr">
@@ -6153,7 +6153,7 @@
       </c>
       <c r="J64" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K64" s="11" t="inlineStr">
@@ -6163,12 +6163,12 @@
       </c>
       <c r="L64" t="inlineStr">
         <is>
-          <t>MP_E33_1B_DY20_R1.fastq.gz</t>
+          <t>E33.1B.DY20-12_Machida18S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M64" t="inlineStr">
         <is>
-          <t>MP_E33_1B_DY20_R2.fastq.gz</t>
+          <t>E33.1B.DY20-12_Machida18S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R64" t="inlineStr">
@@ -6230,7 +6230,7 @@
       </c>
       <c r="J65" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K65" s="11" t="inlineStr">
@@ -6240,12 +6240,12 @@
       </c>
       <c r="L65" t="inlineStr">
         <is>
-          <t>MP_E34_1B_DY20_R1.fastq.gz</t>
+          <t>E34.1B.DY20-12_Machida18S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M65" t="inlineStr">
         <is>
-          <t>MP_E34_1B_DY20_R2.fastq.gz</t>
+          <t>E34.1B.DY20-12_Machida18S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R65" t="inlineStr">
@@ -6307,7 +6307,7 @@
       </c>
       <c r="J66" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K66" s="11" t="inlineStr">
@@ -6317,12 +6317,12 @@
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>MP_E35_1B_DY20_R1.fastq.gz</t>
+          <t>E35.1B.DY20-12_Machida18S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M66" t="inlineStr">
         <is>
-          <t>MP_E35_1B_DY20_R2.fastq.gz</t>
+          <t>E35.1B.DY20-12_Machida18S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R66" t="inlineStr">
@@ -6384,7 +6384,7 @@
       </c>
       <c r="J67" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K67" s="11" t="inlineStr">
@@ -6394,12 +6394,12 @@
       </c>
       <c r="L67" t="inlineStr">
         <is>
-          <t>MP_E36_1B_DY20_R1.fastq.gz</t>
+          <t>E36.1B.DY20-12_Machida18S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M67" t="inlineStr">
         <is>
-          <t>MP_E36_1B_DY20_R2.fastq.gz</t>
+          <t>E36.1B.DY20-12_Machida18S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R67" t="inlineStr">
@@ -6456,7 +6456,7 @@
       </c>
       <c r="J68" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K68" s="11" t="inlineStr">
@@ -6466,12 +6466,12 @@
       </c>
       <c r="L68" t="inlineStr">
         <is>
-          <t>MP_E36_2B_DY20_R1.fastq.gz</t>
+          <t>E36.2B.DY20-12_Machida18S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M68" t="inlineStr">
         <is>
-          <t>MP_E36_2B_DY20_R2.fastq.gz</t>
+          <t>E36.2B.DY20-12_Machida18S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R68" t="inlineStr">
@@ -6533,7 +6533,7 @@
       </c>
       <c r="J69" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K69" s="11" t="inlineStr">
@@ -6543,12 +6543,12 @@
       </c>
       <c r="L69" t="inlineStr">
         <is>
-          <t>MP_E37_1B_DY20_R1.fastq.gz</t>
+          <t>E37.1B.DY20-12_Machida18S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M69" t="inlineStr">
         <is>
-          <t>MP_E37_1B_DY20_R2.fastq.gz</t>
+          <t>E37.1B.DY20-12_Machida18S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R69" t="inlineStr">
@@ -6610,7 +6610,7 @@
       </c>
       <c r="J70" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K70" s="11" t="inlineStr">
@@ -6620,12 +6620,12 @@
       </c>
       <c r="L70" t="inlineStr">
         <is>
-          <t>MP_E38_1B_DY20_R1.fastq.gz</t>
+          <t>E38.1B.DY20-12_Machida18S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M70" t="inlineStr">
         <is>
-          <t>MP_E38_1B_DY20_R2.fastq.gz</t>
+          <t>E38.1B.DY20-12_Machida18S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R70" t="inlineStr">
@@ -6687,7 +6687,7 @@
       </c>
       <c r="J71" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K71" s="11" t="inlineStr">
@@ -6697,12 +6697,12 @@
       </c>
       <c r="L71" t="inlineStr">
         <is>
-          <t>MP_E39_1B_DY20_R1.fastq.gz</t>
+          <t>E39.1B.DY20-12_Machida18S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M71" t="inlineStr">
         <is>
-          <t>MP_E39_1B_DY20_R2.fastq.gz</t>
+          <t>E39.1B.DY20-12_Machida18S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R71" t="inlineStr">
@@ -6764,7 +6764,7 @@
       </c>
       <c r="J72" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K72" s="11" t="inlineStr">
@@ -6774,12 +6774,12 @@
       </c>
       <c r="L72" t="inlineStr">
         <is>
-          <t>MP_E40_1B_DY20_R1.fastq.gz</t>
+          <t>E40.1B.DY20-12_Machida18S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M72" t="inlineStr">
         <is>
-          <t>MP_E40_1B_DY20_R2.fastq.gz</t>
+          <t>E40.1B.DY20-12_Machida18S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R72" t="inlineStr">
@@ -6841,7 +6841,7 @@
       </c>
       <c r="J73" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K73" s="11" t="inlineStr">
@@ -6851,12 +6851,12 @@
       </c>
       <c r="L73" t="inlineStr">
         <is>
-          <t>MP_E42_1B_DY20_R1.fastq.gz</t>
+          <t>E42.1B.DY20-12_Machida18S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M73" t="inlineStr">
         <is>
-          <t>MP_E42_1B_DY20_R2.fastq.gz</t>
+          <t>E42.1B.DY20-12_Machida18S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R73" t="inlineStr">
@@ -6918,7 +6918,7 @@
       </c>
       <c r="J74" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K74" s="11" t="inlineStr">
@@ -6928,12 +6928,12 @@
       </c>
       <c r="L74" t="inlineStr">
         <is>
-          <t>MP_E43_1B_DY20_R1.fastq.gz</t>
+          <t>E43.1B.DY20-12_Machida18S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M74" t="inlineStr">
         <is>
-          <t>MP_E43_1B_DY20_R2.fastq.gz</t>
+          <t>E43.1B.DY20-12_Machida18S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R74" t="inlineStr">
@@ -6995,7 +6995,7 @@
       </c>
       <c r="J75" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K75" s="11" t="inlineStr">
@@ -7005,12 +7005,12 @@
       </c>
       <c r="L75" t="inlineStr">
         <is>
-          <t>MP_E44_DY20_R1.fastq.gz</t>
+          <t>E44.DY20-12_Machida18S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M75" t="inlineStr">
         <is>
-          <t>MP_E44_DY20_R2.fastq.gz</t>
+          <t>E44.DY20-12_Machida18S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R75" t="inlineStr">
@@ -7072,7 +7072,7 @@
       </c>
       <c r="J76" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K76" s="11" t="inlineStr">
@@ -7082,12 +7082,12 @@
       </c>
       <c r="L76" t="inlineStr">
         <is>
-          <t>MP_E45_1B_DY20_R1.fastq.gz</t>
+          <t>E45.1B.DY20-12_Machida18S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M76" t="inlineStr">
         <is>
-          <t>MP_E45_1B_DY20_R2.fastq.gz</t>
+          <t>E45.1B.DY20-12_Machida18S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R76" t="inlineStr">
@@ -7149,7 +7149,7 @@
       </c>
       <c r="J77" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K77" s="11" t="inlineStr">
@@ -7159,12 +7159,12 @@
       </c>
       <c r="L77" t="inlineStr">
         <is>
-          <t>MP_E46_1B_DY20_R1.fastq.gz</t>
+          <t>E46.1B.DY20-12_Machida18S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M77" t="inlineStr">
         <is>
-          <t>MP_E46_1B_DY20_R2.fastq.gz</t>
+          <t>E46.1B.DY20-12_Machida18S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R77" t="inlineStr">
@@ -7226,7 +7226,7 @@
       </c>
       <c r="J78" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K78" s="11" t="inlineStr">
@@ -7236,12 +7236,12 @@
       </c>
       <c r="L78" t="inlineStr">
         <is>
-          <t>MP_E46_2B_DY20_R1.fastq.gz</t>
+          <t>E46.2B.DY20-12_Machida18S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M78" t="inlineStr">
         <is>
-          <t>MP_E46_2B_DY20_R2.fastq.gz</t>
+          <t>E46.2B.DY20-12_Machida18S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R78" t="inlineStr">
@@ -7298,7 +7298,7 @@
       </c>
       <c r="J79" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K79" s="11" t="inlineStr">
@@ -7308,12 +7308,12 @@
       </c>
       <c r="L79" t="inlineStr">
         <is>
-          <t>MP_E47_1B_DY20_R1.fastq.gz</t>
+          <t>E47.1B.DY20-12_Machida18S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M79" t="inlineStr">
         <is>
-          <t>MP_E47_1B_DY20_R2.fastq.gz</t>
+          <t>E47.1B.DY20-12_Machida18S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R79" t="inlineStr">
@@ -7375,7 +7375,7 @@
       </c>
       <c r="J80" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K80" s="11" t="inlineStr">
@@ -7385,12 +7385,12 @@
       </c>
       <c r="L80" t="inlineStr">
         <is>
-          <t>MP_E48_1B_DY20_R1.fastq.gz</t>
+          <t>E48.1B.DY20-12_Machida18S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M80" t="inlineStr">
         <is>
-          <t>MP_E48_1B_DY20_R2.fastq.gz</t>
+          <t>E48.1B.DY20-12_Machida18S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R80" t="inlineStr">
@@ -7452,7 +7452,7 @@
       </c>
       <c r="J81" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K81" s="11" t="inlineStr">
@@ -7462,12 +7462,12 @@
       </c>
       <c r="L81" t="inlineStr">
         <is>
-          <t>MP_E49_1B_DY20_R1.fastq.gz</t>
+          <t>E49.1B.DY20-12_Machida18S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M81" t="inlineStr">
         <is>
-          <t>MP_E49_1B_DY20_R2.fastq.gz</t>
+          <t>E49.1B.DY20-12_Machida18S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R81" t="inlineStr">
@@ -7524,7 +7524,7 @@
       </c>
       <c r="J82" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K82" s="11" t="inlineStr">
@@ -7534,12 +7534,12 @@
       </c>
       <c r="L82" t="inlineStr">
         <is>
-          <t>MP_E49_2B_DY20_R1.fastq.gz</t>
+          <t>E49.2B.DY20-12_Machida18S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M82" t="inlineStr">
         <is>
-          <t>MP_E49_2B_DY20_R2.fastq.gz</t>
+          <t>E49.2B.DY20-12_Machida18S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R82" t="inlineStr">
@@ -7601,7 +7601,7 @@
       </c>
       <c r="J83" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K83" s="11" t="inlineStr">
@@ -7611,12 +7611,12 @@
       </c>
       <c r="L83" t="inlineStr">
         <is>
-          <t>MP_E50_1B_DY20_R1.fastq.gz</t>
+          <t>E50.1B.DY20-12_Machida18S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M83" t="inlineStr">
         <is>
-          <t>MP_E50_1B_DY20_R2.fastq.gz</t>
+          <t>E50.1B.DY20-12_Machida18S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R83" t="inlineStr">
@@ -7678,7 +7678,7 @@
       </c>
       <c r="J84" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K84" s="11" t="inlineStr">
@@ -7688,12 +7688,12 @@
       </c>
       <c r="L84" t="inlineStr">
         <is>
-          <t>MP_E51_1B_DY20_R1.fastq.gz</t>
+          <t>E51.1B.DY20-12_Machida18S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M84" t="inlineStr">
         <is>
-          <t>MP_E51_1B_DY20_R2.fastq.gz</t>
+          <t>E51.1B.DY20-12_Machida18S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R84" t="inlineStr">
@@ -7755,7 +7755,7 @@
       </c>
       <c r="J85" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K85" s="11" t="inlineStr">
@@ -7765,12 +7765,12 @@
       </c>
       <c r="L85" t="inlineStr">
         <is>
-          <t>MP_E52_1B_DY20_R1.fastq.gz</t>
+          <t>E52.1B.DY20-12_Machida18S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M85" t="inlineStr">
         <is>
-          <t>MP_E52_1B_DY20_R2.fastq.gz</t>
+          <t>E52.1B.DY20-12_Machida18S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R85" t="inlineStr">
@@ -7832,7 +7832,7 @@
       </c>
       <c r="J86" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K86" s="11" t="inlineStr">
@@ -7842,12 +7842,12 @@
       </c>
       <c r="L86" t="inlineStr">
         <is>
-          <t>MP_E53_1B_DY20_R1.fastq.gz</t>
+          <t>E53.1B.DY20-12_Machida18S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M86" t="inlineStr">
         <is>
-          <t>MP_E53_1B_DY20_R2.fastq.gz</t>
+          <t>E53.1B.DY20-12_Machida18S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R86" t="inlineStr">
@@ -7904,7 +7904,7 @@
       </c>
       <c r="J87" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K87" s="11" t="inlineStr">
@@ -7914,12 +7914,12 @@
       </c>
       <c r="L87" t="inlineStr">
         <is>
-          <t>MP_E53_2B_DY20_R1.fastq.gz</t>
+          <t>E53.2B.DY20-12_Machida18S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M87" t="inlineStr">
         <is>
-          <t>MP_E53_2B_DY20_R2.fastq.gz</t>
+          <t>E53.2B.DY20-12_Machida18S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R87" t="inlineStr">
@@ -7981,7 +7981,7 @@
       </c>
       <c r="J88" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K88" s="11" t="inlineStr">
@@ -7991,12 +7991,12 @@
       </c>
       <c r="L88" t="inlineStr">
         <is>
-          <t>MP_E54_1B_DY20_R1.fastq.gz</t>
+          <t>E54.1B.DY20-12_Machida18S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M88" t="inlineStr">
         <is>
-          <t>MP_E54_1B_DY20_R2.fastq.gz</t>
+          <t>E54.1B.DY20-12_Machida18S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R88" t="inlineStr">
@@ -8053,7 +8053,7 @@
       </c>
       <c r="J89" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K89" s="11" t="inlineStr">
@@ -8063,12 +8063,12 @@
       </c>
       <c r="L89" t="inlineStr">
         <is>
-          <t>MP_E54_2B_DY20_R1.fastq.gz</t>
+          <t>E54.2B.DY20-12_Machida18S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M89" t="inlineStr">
         <is>
-          <t>MP_E54_2B_DY20_R2.fastq.gz</t>
+          <t>E54.2B.DY20-12_Machida18S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R89" t="inlineStr">
@@ -8130,7 +8130,7 @@
       </c>
       <c r="J90" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K90" s="11" t="inlineStr">
@@ -8140,12 +8140,12 @@
       </c>
       <c r="L90" t="inlineStr">
         <is>
-          <t>MP_E55_1B_DY20_R1.fastq.gz</t>
+          <t>E55.1B.DY20-12_Machida18S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M90" t="inlineStr">
         <is>
-          <t>MP_E55_1B_DY20_R2.fastq.gz</t>
+          <t>E55.1B.DY20-12_Machida18S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R90" t="inlineStr">
@@ -8207,7 +8207,7 @@
       </c>
       <c r="J91" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K91" s="11" t="inlineStr">
@@ -8217,12 +8217,12 @@
       </c>
       <c r="L91" t="inlineStr">
         <is>
-          <t>MP_E57_1B_DY20_R1.fastq.gz</t>
+          <t>E57.1B.DY20-12_Machida18S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M91" t="inlineStr">
         <is>
-          <t>MP_E57_1B_DY20_R2.fastq.gz</t>
+          <t>E57.1B.DY20-12_Machida18S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R91" t="inlineStr">
@@ -8284,7 +8284,7 @@
       </c>
       <c r="J92" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K92" s="11" t="inlineStr">
@@ -8294,12 +8294,12 @@
       </c>
       <c r="L92" t="inlineStr">
         <is>
-          <t>MP_E58_1B_DY20_R1.fastq.gz</t>
+          <t>E58.1B.DY20-12_Machida18S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M92" t="inlineStr">
         <is>
-          <t>MP_E58_1B_DY20_R2.fastq.gz</t>
+          <t>E58.1B.DY20-12_Machida18S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R92" t="inlineStr">
@@ -8356,7 +8356,7 @@
       </c>
       <c r="J93" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K93" s="11" t="inlineStr">
@@ -8366,12 +8366,12 @@
       </c>
       <c r="L93" t="inlineStr">
         <is>
-          <t>MP_E58_2B_DY20_R1.fastq.gz</t>
+          <t>E58.2B.DY20-12_Machida18S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M93" t="inlineStr">
         <is>
-          <t>MP_E58_2B_DY20_R2.fastq.gz</t>
+          <t>E58.2B.DY20-12_Machida18S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R93" t="inlineStr">
@@ -8433,7 +8433,7 @@
       </c>
       <c r="J94" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K94" s="11" t="inlineStr">
@@ -8443,12 +8443,12 @@
       </c>
       <c r="L94" t="inlineStr">
         <is>
-          <t>MP_E59_1B_DY20_R1.fastq.gz</t>
+          <t>E59.1B.DY20-12_Machida18S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M94" t="inlineStr">
         <is>
-          <t>MP_E59_1B_DY20_R2.fastq.gz</t>
+          <t>E59.1B.DY20-12_Machida18S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R94" t="inlineStr">
@@ -8510,7 +8510,7 @@
       </c>
       <c r="J95" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K95" s="11" t="inlineStr">
@@ -8520,12 +8520,12 @@
       </c>
       <c r="L95" t="inlineStr">
         <is>
-          <t>MP_E60_1B_DY20_R1.fastq.gz</t>
+          <t>E60.1B.DY20-12_Machida18S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M95" t="inlineStr">
         <is>
-          <t>MP_E60_1B_DY20_R2.fastq.gz</t>
+          <t>E60.1B.DY20-12_Machida18S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R95" t="inlineStr">
@@ -8587,7 +8587,7 @@
       </c>
       <c r="J96" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K96" s="11" t="inlineStr">
@@ -8597,12 +8597,12 @@
       </c>
       <c r="L96" t="inlineStr">
         <is>
-          <t>MP_E61_1B_DY20_R1.fastq.gz</t>
+          <t>E61.1B.DY20-12_Machida18S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M96" t="inlineStr">
         <is>
-          <t>MP_E61_1B_DY20_R2.fastq.gz</t>
+          <t>E61.1B.DY20-12_Machida18S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R96" t="inlineStr">
@@ -8664,7 +8664,7 @@
       </c>
       <c r="J97" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K97" s="11" t="inlineStr">
@@ -8674,12 +8674,12 @@
       </c>
       <c r="L97" t="inlineStr">
         <is>
-          <t>MP_E62_1B_DY20_R1.fastq.gz</t>
+          <t>E62.1B.DY20-12_Machida18S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M97" t="inlineStr">
         <is>
-          <t>MP_E62_1B_DY20_R2.fastq.gz</t>
+          <t>E62.1B.DY20-12_Machida18S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R97" t="inlineStr">
@@ -8741,7 +8741,7 @@
       </c>
       <c r="J98" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K98" s="11" t="inlineStr">
@@ -8751,12 +8751,12 @@
       </c>
       <c r="L98" t="inlineStr">
         <is>
-          <t>MP_E63_1B_DY20_R1.fastq.gz</t>
+          <t>E63.1B.DY20-12_Machida18S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M98" t="inlineStr">
         <is>
-          <t>MP_E63_1B_DY20_R2.fastq.gz</t>
+          <t>E63.1B.DY20-12_Machida18S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R98" t="inlineStr">
@@ -8818,7 +8818,7 @@
       </c>
       <c r="J99" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K99" s="11" t="inlineStr">
@@ -8828,12 +8828,12 @@
       </c>
       <c r="L99" t="inlineStr">
         <is>
-          <t>MP_E64_1B_DY20_R1.fastq.gz</t>
+          <t>E64.1B.DY20-12_Machida18S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M99" t="inlineStr">
         <is>
-          <t>MP_E64_1B_DY20_R2.fastq.gz</t>
+          <t>E64.1B.DY20-12_Machida18S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R99" t="inlineStr">
@@ -8895,7 +8895,7 @@
       </c>
       <c r="J100" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K100" s="11" t="inlineStr">
@@ -8905,12 +8905,12 @@
       </c>
       <c r="L100" t="inlineStr">
         <is>
-          <t>MP_E65_1B_DY20_R1.fastq.gz</t>
+          <t>E65.1B.DY20-12_Machida18S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M100" t="inlineStr">
         <is>
-          <t>MP_E65_1B_DY20_R2.fastq.gz</t>
+          <t>E65.1B.DY20-12_Machida18S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R100" t="inlineStr">
@@ -8972,7 +8972,7 @@
       </c>
       <c r="J101" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K101" s="11" t="inlineStr">
@@ -8982,12 +8982,12 @@
       </c>
       <c r="L101" t="inlineStr">
         <is>
-          <t>MP_E66_1B_DY20_R1.fastq.gz</t>
+          <t>E66.1B.DY20-12_Machida18S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M101" t="inlineStr">
         <is>
-          <t>MP_E66_1B_DY20_R2.fastq.gz</t>
+          <t>E66.1B.DY20-12_Machida18S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R101" t="inlineStr">
@@ -9049,7 +9049,7 @@
       </c>
       <c r="J102" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K102" s="11" t="inlineStr">
@@ -9059,12 +9059,12 @@
       </c>
       <c r="L102" t="inlineStr">
         <is>
-          <t>MP_E67_1B_DY20_R1.fastq.gz</t>
+          <t>E67.1B.DY20-12_Machida18S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M102" t="inlineStr">
         <is>
-          <t>MP_E67_1B_DY20_R2.fastq.gz</t>
+          <t>E67.1B.DY20-12_Machida18S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R102" t="inlineStr">
@@ -9126,7 +9126,7 @@
       </c>
       <c r="J103" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K103" s="11" t="inlineStr">
@@ -9136,12 +9136,12 @@
       </c>
       <c r="L103" t="inlineStr">
         <is>
-          <t>MP_E68_1B_DY20_R1.fastq.gz</t>
+          <t>E68.1B.DY20-12_Machida18S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M103" t="inlineStr">
         <is>
-          <t>MP_E68_1B_DY20_R2.fastq.gz</t>
+          <t>E68.1B.DY20-12_Machida18S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R103" t="inlineStr">
@@ -9203,7 +9203,7 @@
       </c>
       <c r="J104" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K104" s="11" t="inlineStr">
@@ -9213,12 +9213,12 @@
       </c>
       <c r="L104" t="inlineStr">
         <is>
-          <t>MP_E69_1B_DY20_R1.fastq.gz</t>
+          <t>E69.1B.DY20-12_Machida18S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M104" t="inlineStr">
         <is>
-          <t>MP_E69_1B_DY20_R2.fastq.gz</t>
+          <t>E69.1B.DY20-12_Machida18S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R104" t="inlineStr">
@@ -9280,7 +9280,7 @@
       </c>
       <c r="J105" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K105" s="11" t="inlineStr">
@@ -9290,12 +9290,12 @@
       </c>
       <c r="L105" t="inlineStr">
         <is>
-          <t>MP_E70_1B_DY20_R1.fastq.gz</t>
+          <t>E70.1B.DY20-12_Machida18S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M105" t="inlineStr">
         <is>
-          <t>MP_E70_1B_DY20_R2.fastq.gz</t>
+          <t>E70.1B.DY20-12_Machida18S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R105" t="inlineStr">
@@ -9357,7 +9357,7 @@
       </c>
       <c r="J106" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K106" s="11" t="inlineStr">
@@ -9367,12 +9367,12 @@
       </c>
       <c r="L106" t="inlineStr">
         <is>
-          <t>MP_E71_1B_DY20_R1.fastq.gz</t>
+          <t>E71.1B.DY20-12_Machida18S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M106" t="inlineStr">
         <is>
-          <t>MP_E71_1B_DY20_R2.fastq.gz</t>
+          <t>E71.1B.DY20-12_Machida18S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R106" t="inlineStr">
@@ -9434,7 +9434,7 @@
       </c>
       <c r="J107" t="inlineStr">
         <is>
-          <t>Sequencing performed at None</t>
+          <t>Sequencing performed at Oregon State University Center for Quantitative Life Sciences Genomics Core</t>
         </is>
       </c>
       <c r="K107" s="11" t="inlineStr">
@@ -9444,12 +9444,12 @@
       </c>
       <c r="L107" t="inlineStr">
         <is>
-          <t>MP_E72_1B_DY20_R1.fastq.gz</t>
+          <t>E72.1B.DY20-12_Machida18S_osu867_R1.fastq.gz</t>
         </is>
       </c>
       <c r="M107" t="inlineStr">
         <is>
-          <t>MP_E72_1B_DY20_R2.fastq.gz</t>
+          <t>E72.1B.DY20-12_Machida18S_osu867_R2.fastq.gz</t>
         </is>
       </c>
       <c r="R107" t="inlineStr">

</xml_diff>